<commit_message>
reorganize analyzer files. add script to assign volume and surface area.
</commit_message>
<xml_diff>
--- a/field_notes/BlueFlux Dataset_soils_water.xlsx
+++ b/field_notes/BlueFlux Dataset_soils_water.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jongewirtzman/My Drive/Research/Blueflux/blueflux-ground/field_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE107C62-5307-2542-8289-C44638145005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4AE6E8-7909-6D4C-8BBF-6558020AE5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37160" yWindow="-6020" windowWidth="30240" windowHeight="17300" xr2:uid="{CBF0C425-0157-C64F-9486-00F0554822BF}"/>
+    <workbookView xWindow="15860" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CBF0C425-0157-C64F-9486-00F0554822BF}"/>
   </bookViews>
   <sheets>
     <sheet name="soil flux data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="181">
   <si>
     <t>Plot</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>no visible bubbles once tide has come in a bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Water 11</t>
+  </si>
+  <si>
+    <t>Water 12</t>
   </si>
 </sst>
 </file>
@@ -957,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515189A3-083C-2248-820C-6CDC4714B802}">
-  <dimension ref="A1:T100"/>
+  <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="82" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2643,7 +2652,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2696,7 +2705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2749,7 +2758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2802,122 +2811,76 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>45263</v>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>179</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.65763888888888888</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G37">
-        <v>23.9</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="G37" t="s">
+        <v>53</v>
       </c>
       <c r="I37" s="1">
-        <v>0.47222222222222221</v>
+        <v>0.67777777777777781</v>
       </c>
       <c r="J37" s="1">
-        <v>0.47708333333333336</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L37">
-        <v>24.9</v>
-      </c>
-      <c r="M37">
-        <v>24.7</v>
-      </c>
-      <c r="N37">
-        <v>1016</v>
-      </c>
-      <c r="O37">
-        <v>1016.1</v>
-      </c>
-      <c r="P37">
-        <v>65.5</v>
-      </c>
-      <c r="Q37">
-        <v>68</v>
-      </c>
-      <c r="R37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <v>45263</v>
-      </c>
-      <c r="B38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38">
-        <v>23</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="J38" s="1">
-        <v>0.48055555555555557</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L38">
-        <v>24.4</v>
-      </c>
-      <c r="M38">
-        <v>24.5</v>
-      </c>
-      <c r="N38">
-        <v>1016.1</v>
-      </c>
-      <c r="O38">
-        <v>1016.1</v>
-      </c>
-      <c r="P38">
-        <v>68.2</v>
-      </c>
-      <c r="Q38">
-        <v>73.8</v>
-      </c>
-      <c r="R38" t="s">
-        <v>97</v>
-      </c>
-      <c r="T38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+        <v>0.67986111111111114</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="Z37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>45263</v>
       </c>
@@ -2925,10 +2888,10 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -2937,46 +2900,43 @@
         <v>83</v>
       </c>
       <c r="G39">
-        <v>23.5</v>
+        <v>23.9</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" s="1">
-        <v>0.48334490740740743</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="J39" s="1">
-        <v>0.48472222222222222</v>
+        <v>0.47708333333333336</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L39" t="s">
-        <v>12</v>
-      </c>
-      <c r="M39" t="s">
-        <v>12</v>
-      </c>
-      <c r="N39" t="s">
-        <v>12</v>
-      </c>
-      <c r="O39" t="s">
-        <v>12</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>12</v>
+      <c r="L39">
+        <v>24.9</v>
+      </c>
+      <c r="M39">
+        <v>24.7</v>
+      </c>
+      <c r="N39">
+        <v>1016</v>
+      </c>
+      <c r="O39">
+        <v>1016.1</v>
+      </c>
+      <c r="P39">
+        <v>65.5</v>
+      </c>
+      <c r="Q39">
+        <v>68</v>
       </c>
       <c r="R39" t="s">
         <v>97</v>
       </c>
-      <c r="T39" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>45263</v>
       </c>
@@ -2984,7 +2944,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D40" t="s">
         <v>67</v>
@@ -2996,46 +2956,46 @@
         <v>83</v>
       </c>
       <c r="G40">
-        <v>23.7</v>
+        <v>23</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40" s="1">
-        <v>0.49444444444444446</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="J40" s="1">
-        <v>0.49583333333333335</v>
+        <v>0.48055555555555557</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L40" t="s">
-        <v>12</v>
-      </c>
-      <c r="M40" t="s">
-        <v>12</v>
-      </c>
-      <c r="N40" t="s">
-        <v>12</v>
-      </c>
-      <c r="O40" t="s">
-        <v>12</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>12</v>
+      <c r="L40">
+        <v>24.4</v>
+      </c>
+      <c r="M40">
+        <v>24.5</v>
+      </c>
+      <c r="N40">
+        <v>1016.1</v>
+      </c>
+      <c r="O40">
+        <v>1016.1</v>
+      </c>
+      <c r="P40">
+        <v>68.2</v>
+      </c>
+      <c r="Q40">
+        <v>73.8</v>
       </c>
       <c r="R40" t="s">
         <v>97</v>
       </c>
       <c r="T40" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>45263</v>
       </c>
@@ -3043,10 +3003,10 @@
         <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -3061,51 +3021,51 @@
         <v>0</v>
       </c>
       <c r="I41" s="1">
-        <v>0.50138888888888888</v>
+        <v>0.48334490740740743</v>
       </c>
       <c r="J41" s="1">
-        <v>0.50347222222222221</v>
+        <v>0.48472222222222222</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L41">
-        <v>25.1</v>
-      </c>
-      <c r="M41">
-        <v>25.4</v>
-      </c>
-      <c r="N41">
-        <v>1016.2</v>
-      </c>
-      <c r="O41">
-        <v>1016.2</v>
-      </c>
-      <c r="P41">
-        <v>68.599999999999994</v>
-      </c>
-      <c r="Q41">
-        <v>74.5</v>
+      <c r="L41" t="s">
+        <v>12</v>
+      </c>
+      <c r="M41" t="s">
+        <v>12</v>
+      </c>
+      <c r="N41" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" t="s">
+        <v>12</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="R41" t="s">
         <v>97</v>
       </c>
       <c r="T41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45263</v>
       </c>
       <c r="B42" t="s">
         <v>60</v>
       </c>
-      <c r="C42">
-        <v>6</v>
+      <c r="C42" t="s">
+        <v>64</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -3114,54 +3074,57 @@
         <v>83</v>
       </c>
       <c r="G42">
-        <v>23.5</v>
+        <v>23.7</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42" s="1">
-        <v>0.50763888888888886</v>
+        <v>0.49444444444444446</v>
       </c>
       <c r="J42" s="1">
-        <v>0.50902777777777775</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L42">
-        <v>25.2</v>
-      </c>
-      <c r="M42">
-        <v>25.4</v>
-      </c>
-      <c r="N42">
-        <v>1015.8</v>
-      </c>
-      <c r="O42">
-        <v>1015.9</v>
-      </c>
-      <c r="P42">
-        <v>73.3</v>
-      </c>
-      <c r="Q42">
-        <v>75.5</v>
+      <c r="L42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N42" t="s">
+        <v>12</v>
+      </c>
+      <c r="O42" t="s">
+        <v>12</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="R42" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>45263</v>
       </c>
       <c r="B43" t="s">
         <v>60</v>
       </c>
-      <c r="C43">
-        <v>7</v>
+      <c r="C43" t="s">
+        <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -3176,37 +3139,40 @@
         <v>0</v>
       </c>
       <c r="I43" s="1">
-        <v>0.5131944444444444</v>
+        <v>0.50138888888888888</v>
       </c>
       <c r="J43" s="1">
-        <v>0.51458333333333328</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L43">
+        <v>25.1</v>
+      </c>
+      <c r="M43">
         <v>25.4</v>
       </c>
-      <c r="M43">
-        <v>25.8</v>
-      </c>
       <c r="N43">
-        <v>1016</v>
+        <v>1016.2</v>
       </c>
       <c r="O43">
-        <v>1015.9</v>
+        <v>1016.2</v>
       </c>
       <c r="P43">
-        <v>70.400000000000006</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="Q43">
-        <v>78.2</v>
+        <v>74.5</v>
       </c>
       <c r="R43" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>45263</v>
       </c>
@@ -3214,10 +3180,10 @@
         <v>60</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -3226,43 +3192,43 @@
         <v>83</v>
       </c>
       <c r="G44">
-        <v>23.6</v>
+        <v>23.5</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44" s="1">
-        <v>0.51840277777777777</v>
+        <v>0.50763888888888886</v>
       </c>
       <c r="J44" s="1">
-        <v>0.51979166666666665</v>
+        <v>0.50902777777777775</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L44">
-        <v>25.9</v>
+        <v>25.2</v>
       </c>
       <c r="M44">
-        <v>26</v>
+        <v>25.4</v>
       </c>
       <c r="N44">
-        <v>1016</v>
+        <v>1015.8</v>
       </c>
       <c r="O44">
-        <v>1016</v>
+        <v>1015.9</v>
       </c>
       <c r="P44">
-        <v>75.2</v>
+        <v>73.3</v>
       </c>
       <c r="Q44">
-        <v>78.5</v>
+        <v>75.5</v>
       </c>
       <c r="R44" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>45263</v>
       </c>
@@ -3270,10 +3236,10 @@
         <v>60</v>
       </c>
       <c r="C45">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -3288,37 +3254,37 @@
         <v>0</v>
       </c>
       <c r="I45" s="1">
-        <v>0.52500000000000002</v>
+        <v>0.5131944444444444</v>
       </c>
       <c r="J45" s="1">
-        <v>0.52638888888888891</v>
+        <v>0.51458333333333328</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L45">
-        <v>27</v>
+        <v>25.4</v>
       </c>
       <c r="M45">
-        <v>27.7</v>
+        <v>25.8</v>
       </c>
       <c r="N45">
-        <v>1017.3</v>
+        <v>1016</v>
       </c>
       <c r="O45">
-        <v>1016.9</v>
+        <v>1015.9</v>
       </c>
       <c r="P45">
-        <v>74.900000000000006</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="Q45">
-        <v>78.5</v>
+        <v>78.2</v>
       </c>
       <c r="R45" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45263</v>
       </c>
@@ -3326,10 +3292,10 @@
         <v>60</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -3338,43 +3304,43 @@
         <v>83</v>
       </c>
       <c r="G46">
-        <v>23.5</v>
-      </c>
-      <c r="H46" t="s">
-        <v>88</v>
+        <v>23.6</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
       </c>
       <c r="I46" s="1">
-        <v>0.53194444444444444</v>
+        <v>0.51840277777777777</v>
       </c>
       <c r="J46" s="1">
-        <v>0.53333333333333333</v>
+        <v>0.51979166666666665</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L46">
-        <v>26.8</v>
+        <v>25.9</v>
       </c>
       <c r="M46">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N46">
-        <v>1015.3</v>
+        <v>1016</v>
       </c>
       <c r="O46">
-        <v>1013.3</v>
+        <v>1016</v>
       </c>
       <c r="P46">
-        <v>69.8</v>
+        <v>75.2</v>
       </c>
       <c r="Q46">
-        <v>73.400000000000006</v>
+        <v>78.5</v>
       </c>
       <c r="R46" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>45263</v>
       </c>
@@ -3382,10 +3348,10 @@
         <v>60</v>
       </c>
       <c r="C47">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -3394,43 +3360,43 @@
         <v>83</v>
       </c>
       <c r="G47">
-        <v>23.4</v>
-      </c>
-      <c r="H47" t="s">
-        <v>88</v>
+        <v>23.5</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
       </c>
       <c r="I47" s="1">
-        <v>0.53749999999999998</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="J47" s="1">
-        <v>0.53888888888888886</v>
+        <v>0.52638888888888891</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L47">
-        <v>27.4</v>
+        <v>27</v>
       </c>
       <c r="M47">
-        <v>28.7</v>
+        <v>27.7</v>
       </c>
       <c r="N47">
-        <v>1016.4</v>
+        <v>1017.3</v>
       </c>
       <c r="O47">
-        <v>1016.6</v>
+        <v>1016.9</v>
       </c>
       <c r="P47">
-        <v>92.6</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="Q47">
-        <v>76.5</v>
+        <v>78.5</v>
       </c>
       <c r="R47" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>45263</v>
       </c>
@@ -3438,10 +3404,10 @@
         <v>60</v>
       </c>
       <c r="C48">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -3450,43 +3416,40 @@
         <v>83</v>
       </c>
       <c r="G48">
-        <v>23.3</v>
+        <v>23.5</v>
       </c>
       <c r="H48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I48" s="1">
-        <v>0.54409722222222223</v>
+        <v>0.53194444444444444</v>
       </c>
       <c r="J48" s="1">
-        <v>0.54548611111111112</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L48" t="s">
-        <v>12</v>
-      </c>
-      <c r="M48" t="s">
-        <v>12</v>
-      </c>
-      <c r="N48" t="s">
-        <v>12</v>
-      </c>
-      <c r="O48" t="s">
-        <v>12</v>
-      </c>
-      <c r="P48" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>12</v>
+      <c r="L48">
+        <v>26.8</v>
+      </c>
+      <c r="M48">
+        <v>27</v>
+      </c>
+      <c r="N48">
+        <v>1015.3</v>
+      </c>
+      <c r="O48">
+        <v>1013.3</v>
+      </c>
+      <c r="P48">
+        <v>69.8</v>
+      </c>
+      <c r="Q48">
+        <v>73.400000000000006</v>
       </c>
       <c r="R48" t="s">
         <v>97</v>
-      </c>
-      <c r="T48" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
@@ -3497,10 +3460,10 @@
         <v>60</v>
       </c>
       <c r="C49">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -3509,43 +3472,40 @@
         <v>83</v>
       </c>
       <c r="G49">
-        <v>24.8</v>
+        <v>23.4</v>
       </c>
       <c r="H49" t="s">
         <v>88</v>
       </c>
       <c r="I49" s="1">
-        <v>0.54791666666666672</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="J49" s="1">
-        <v>0.5493055555555556</v>
+        <v>0.53888888888888886</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L49">
-        <v>26.7</v>
+        <v>27.4</v>
       </c>
       <c r="M49">
-        <v>27</v>
+        <v>28.7</v>
       </c>
       <c r="N49">
-        <v>1014.8</v>
+        <v>1016.4</v>
       </c>
       <c r="O49">
-        <v>1015.2</v>
+        <v>1016.6</v>
       </c>
       <c r="P49">
-        <v>71.8</v>
+        <v>92.6</v>
       </c>
       <c r="Q49">
-        <v>77</v>
+        <v>76.5</v>
       </c>
       <c r="R49" t="s">
         <v>97</v>
-      </c>
-      <c r="T49" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
@@ -3556,10 +3516,10 @@
         <v>60</v>
       </c>
       <c r="C50">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -3568,43 +3528,43 @@
         <v>83</v>
       </c>
       <c r="G50">
-        <v>23.5</v>
+        <v>23.3</v>
       </c>
       <c r="H50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I50" s="1">
-        <v>0.55243055555555554</v>
+        <v>0.54409722222222223</v>
       </c>
       <c r="J50" s="1">
-        <v>0.55381944444444442</v>
+        <v>0.54548611111111112</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L50">
-        <v>26.6</v>
-      </c>
-      <c r="M50">
-        <v>26.8</v>
-      </c>
-      <c r="N50">
-        <v>1015.1</v>
-      </c>
-      <c r="O50">
-        <v>1015.3</v>
-      </c>
-      <c r="P50">
-        <v>72.3</v>
-      </c>
-      <c r="Q50">
-        <v>75.400000000000006</v>
+      <c r="L50" t="s">
+        <v>12</v>
+      </c>
+      <c r="M50" t="s">
+        <v>12</v>
+      </c>
+      <c r="N50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O50" t="s">
+        <v>12</v>
+      </c>
+      <c r="P50" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>12</v>
       </c>
       <c r="R50" t="s">
         <v>97</v>
       </c>
       <c r="T50" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
@@ -3618,7 +3578,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
@@ -3627,43 +3587,43 @@
         <v>83</v>
       </c>
       <c r="G51">
-        <v>23.1</v>
+        <v>24.8</v>
       </c>
       <c r="H51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I51" s="1">
-        <v>0.55937499999999996</v>
+        <v>0.54791666666666672</v>
       </c>
       <c r="J51" s="1">
-        <v>0.56076388888888884</v>
+        <v>0.5493055555555556</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L51">
-        <v>27.2</v>
+        <v>26.7</v>
       </c>
       <c r="M51">
-        <v>27.3</v>
+        <v>27</v>
       </c>
       <c r="N51">
-        <v>1015.9</v>
+        <v>1014.8</v>
       </c>
       <c r="O51">
-        <v>1015.4</v>
+        <v>1015.2</v>
       </c>
       <c r="P51">
-        <v>70.599999999999994</v>
+        <v>71.8</v>
       </c>
       <c r="Q51">
-        <v>73.5</v>
+        <v>77</v>
       </c>
       <c r="R51" t="s">
         <v>97</v>
       </c>
       <c r="T51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
@@ -3674,10 +3634,10 @@
         <v>60</v>
       </c>
       <c r="C52">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
         <v>13</v>
@@ -3686,40 +3646,43 @@
         <v>83</v>
       </c>
       <c r="G52">
-        <v>23.4</v>
+        <v>23.5</v>
       </c>
       <c r="H52" t="s">
         <v>90</v>
       </c>
       <c r="I52" s="1">
-        <v>0.57013888888888886</v>
+        <v>0.55243055555555554</v>
       </c>
       <c r="J52" s="1">
-        <v>0.57152777777777775</v>
+        <v>0.55381944444444442</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L52">
-        <v>27.2</v>
+        <v>26.6</v>
       </c>
       <c r="M52">
-        <v>27.3</v>
+        <v>26.8</v>
       </c>
       <c r="N52">
-        <v>1015</v>
+        <v>1015.1</v>
       </c>
       <c r="O52">
-        <v>1015</v>
+        <v>1015.3</v>
       </c>
       <c r="P52">
-        <v>69.3</v>
+        <v>72.3</v>
       </c>
       <c r="Q52">
-        <v>73.8</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="R52" t="s">
         <v>97</v>
+      </c>
+      <c r="T52" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
@@ -3729,50 +3692,56 @@
       <c r="B53" t="s">
         <v>60</v>
       </c>
-      <c r="C53" t="s">
-        <v>42</v>
+      <c r="C53">
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G53" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="G53">
+        <v>23.1</v>
       </c>
       <c r="H53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I53" s="1">
-        <v>0.57881944444444444</v>
+        <v>0.55937499999999996</v>
       </c>
       <c r="J53" s="1">
-        <v>0.58576388888888886</v>
+        <v>0.56076388888888884</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L53" t="s">
-        <v>12</v>
-      </c>
-      <c r="M53" t="s">
-        <v>12</v>
-      </c>
-      <c r="N53" t="s">
-        <v>12</v>
-      </c>
-      <c r="O53" t="s">
-        <v>12</v>
-      </c>
-      <c r="P53" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>12</v>
+      <c r="L53">
+        <v>27.2</v>
+      </c>
+      <c r="M53">
+        <v>27.3</v>
+      </c>
+      <c r="N53">
+        <v>1015.9</v>
+      </c>
+      <c r="O53">
+        <v>1015.4</v>
+      </c>
+      <c r="P53">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="Q53">
+        <v>73.5</v>
+      </c>
+      <c r="R53" t="s">
+        <v>97</v>
+      </c>
+      <c r="T53" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -3782,50 +3751,53 @@
       <c r="B54" t="s">
         <v>60</v>
       </c>
-      <c r="C54" t="s">
-        <v>43</v>
+      <c r="C54">
+        <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G54" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="G54">
+        <v>23.4</v>
       </c>
       <c r="H54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I54" s="1">
-        <v>0.59236111111111112</v>
+        <v>0.57013888888888886</v>
       </c>
       <c r="J54" s="1">
-        <v>0.59583333333333333</v>
+        <v>0.57152777777777775</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L54" t="s">
-        <v>12</v>
-      </c>
-      <c r="M54" t="s">
-        <v>12</v>
-      </c>
-      <c r="N54" t="s">
-        <v>12</v>
-      </c>
-      <c r="O54" t="s">
-        <v>12</v>
-      </c>
-      <c r="P54" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>12</v>
+      <c r="L54">
+        <v>27.2</v>
+      </c>
+      <c r="M54">
+        <v>27.3</v>
+      </c>
+      <c r="N54">
+        <v>1015</v>
+      </c>
+      <c r="O54">
+        <v>1015</v>
+      </c>
+      <c r="P54">
+        <v>69.3</v>
+      </c>
+      <c r="Q54">
+        <v>73.8</v>
+      </c>
+      <c r="R54" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
@@ -3836,10 +3808,10 @@
         <v>60</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -3851,13 +3823,13 @@
         <v>85</v>
       </c>
       <c r="H55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55" s="1">
-        <v>0.6</v>
+        <v>0.57881944444444444</v>
       </c>
       <c r="J55" s="1">
-        <v>0.60347222222222219</v>
+        <v>0.58576388888888886</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>12</v>
@@ -3889,10 +3861,10 @@
         <v>60</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -3901,16 +3873,16 @@
         <v>96</v>
       </c>
       <c r="G56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I56" s="1">
-        <v>0.6069444444444444</v>
+        <v>0.59236111111111112</v>
       </c>
       <c r="J56" s="1">
-        <v>0.61041666666666672</v>
+        <v>0.59583333333333333</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>12</v>
@@ -3942,10 +3914,10 @@
         <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D57" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -3954,16 +3926,16 @@
         <v>96</v>
       </c>
       <c r="G57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H57" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I57" s="1">
-        <v>0.6166666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="J57" s="1">
-        <v>0.62013888888888891</v>
+        <v>0.60347222222222219</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>12</v>
@@ -3988,122 +3960,113 @@
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P58" s="2"/>
+      <c r="A58" s="3">
+        <v>45263</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G58" t="s">
+        <v>86</v>
+      </c>
+      <c r="H58" t="s">
+        <v>94</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.61041666666666672</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" t="s">
+        <v>12</v>
+      </c>
+      <c r="M58" t="s">
+        <v>12</v>
+      </c>
+      <c r="N58" t="s">
+        <v>12</v>
+      </c>
+      <c r="O58" t="s">
+        <v>12</v>
+      </c>
+      <c r="P58" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
-        <v>45233</v>
+        <v>45263</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="D59" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="E59" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G59">
-        <v>25.6</v>
+        <v>96</v>
+      </c>
+      <c r="G59" t="s">
+        <v>87</v>
       </c>
       <c r="H59" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="I59" s="1">
-        <v>0.55277777777777781</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="J59" s="1">
-        <v>0.55625000000000002</v>
+        <v>0.62013888888888891</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R59" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="T59" s="2" t="s">
-        <v>98</v>
+      <c r="L59" t="s">
+        <v>12</v>
+      </c>
+      <c r="M59" t="s">
+        <v>12</v>
+      </c>
+      <c r="N59" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" t="s">
+        <v>12</v>
+      </c>
+      <c r="P59" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
-        <v>45233</v>
-      </c>
-      <c r="B60" t="s">
-        <v>105</v>
-      </c>
-      <c r="C60" t="s">
-        <v>107</v>
-      </c>
-      <c r="D60" t="s">
-        <v>110</v>
-      </c>
-      <c r="E60" t="s">
-        <v>112</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G60">
-        <v>25.6</v>
-      </c>
-      <c r="H60" t="s">
-        <v>114</v>
-      </c>
-      <c r="I60" s="1">
-        <v>0.56319444444444444</v>
-      </c>
-      <c r="J60" s="1">
-        <v>0.56736111111111109</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R60" s="2" t="s">
-        <v>177</v>
-      </c>
+      <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
@@ -4113,10 +4076,10 @@
         <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E61" t="s">
         <v>112</v>
@@ -4125,16 +4088,16 @@
         <v>113</v>
       </c>
       <c r="G61">
-        <v>25.7</v>
+        <v>25.6</v>
       </c>
       <c r="H61" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="I61" s="1">
-        <v>0.57291666666666663</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="J61" s="1">
-        <v>0.57638888888888884</v>
+        <v>0.55625000000000002</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>12</v>
@@ -4158,7 +4121,66 @@
         <v>12</v>
       </c>
       <c r="R61" s="2" t="s">
-        <v>54</v>
+        <v>115</v>
+      </c>
+      <c r="T61" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>45233</v>
+      </c>
+      <c r="B62" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" t="s">
+        <v>110</v>
+      </c>
+      <c r="E62" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G62">
+        <v>25.6</v>
+      </c>
+      <c r="H62" t="s">
+        <v>114</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.56319444444444444</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.56736111111111109</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R62" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
@@ -4168,29 +4190,29 @@
       <c r="B63" t="s">
         <v>105</v>
       </c>
-      <c r="C63">
-        <v>1</v>
+      <c r="C63" t="s">
+        <v>108</v>
       </c>
       <c r="D63" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="E63" t="s">
         <v>112</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="G63">
-        <v>24.5</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
+        <v>25.7</v>
+      </c>
+      <c r="H63" t="s">
+        <v>93</v>
       </c>
       <c r="I63" s="1">
-        <v>0.47986111111111113</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="J63" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.57638888888888884</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>12</v>
@@ -4213,58 +4235,8 @@
       <c r="Q63" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
-        <v>45233</v>
-      </c>
-      <c r="B64" t="s">
-        <v>105</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" t="s">
-        <v>112</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G64">
-        <v>25.2</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64" s="1">
-        <v>0.4909722222222222</v>
-      </c>
-      <c r="J64" s="1">
-        <v>0.49236111111111114</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q64" s="2" t="s">
-        <v>12</v>
+      <c r="R63" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
@@ -4275,7 +4247,7 @@
         <v>105</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
         <v>72</v>
@@ -4287,37 +4259,37 @@
         <v>33</v>
       </c>
       <c r="G65">
-        <v>25.2</v>
+        <v>24.5</v>
       </c>
       <c r="H65">
         <v>0</v>
       </c>
       <c r="I65" s="1">
-        <v>0.49479166666666669</v>
+        <v>0.47986111111111113</v>
       </c>
       <c r="J65" s="1">
-        <v>0.49618055555555557</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L65">
-        <v>87.2</v>
-      </c>
-      <c r="M65">
-        <v>87.2</v>
-      </c>
-      <c r="N65">
-        <v>29.98</v>
-      </c>
-      <c r="O65">
-        <v>29.98</v>
-      </c>
-      <c r="P65">
-        <v>61.9</v>
-      </c>
-      <c r="Q65">
-        <v>69.5</v>
+      <c r="L65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q65" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
@@ -4328,10 +4300,10 @@
         <v>105</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="E66" t="s">
         <v>112</v>
@@ -4340,40 +4312,37 @@
         <v>33</v>
       </c>
       <c r="G66">
-        <v>24.3</v>
+        <v>25.2</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <v>0.49965277777777778</v>
+        <v>0.4909722222222222</v>
       </c>
       <c r="J66" s="1">
-        <v>0.50104166666666672</v>
+        <v>0.49236111111111114</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L66">
-        <v>84.2</v>
-      </c>
-      <c r="M66">
-        <v>83.7</v>
-      </c>
-      <c r="N66">
-        <v>29.98</v>
-      </c>
-      <c r="O66">
-        <v>29.98</v>
-      </c>
-      <c r="P66">
-        <v>61.5</v>
-      </c>
-      <c r="Q66">
-        <v>67.5</v>
-      </c>
-      <c r="T66" t="s">
-        <v>98</v>
+      <c r="L66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q66" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
@@ -4384,10 +4353,10 @@
         <v>105</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="E67" t="s">
         <v>112</v>
@@ -4396,25 +4365,25 @@
         <v>33</v>
       </c>
       <c r="G67">
-        <v>24.1</v>
+        <v>25.2</v>
       </c>
       <c r="H67">
         <v>0</v>
       </c>
       <c r="I67" s="1">
-        <v>0.50555555555555554</v>
+        <v>0.49479166666666669</v>
       </c>
       <c r="J67" s="1">
-        <v>0.50694444444444442</v>
+        <v>0.49618055555555557</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L67">
-        <v>81.400000000000006</v>
+        <v>87.2</v>
       </c>
       <c r="M67">
-        <v>81.099999999999994</v>
+        <v>87.2</v>
       </c>
       <c r="N67">
         <v>29.98</v>
@@ -4423,13 +4392,10 @@
         <v>29.98</v>
       </c>
       <c r="P67">
-        <v>69.599999999999994</v>
+        <v>61.9</v>
       </c>
       <c r="Q67">
-        <v>73.2</v>
-      </c>
-      <c r="T67" t="s">
-        <v>120</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
@@ -4440,10 +4406,10 @@
         <v>105</v>
       </c>
       <c r="C68">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E68" t="s">
         <v>112</v>
@@ -4452,25 +4418,25 @@
         <v>33</v>
       </c>
       <c r="G68">
-        <v>24</v>
+        <v>24.3</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="I68" s="1">
-        <v>0.50902777777777775</v>
+        <v>0.49965277777777778</v>
       </c>
       <c r="J68" s="1">
-        <v>0.51041666666666663</v>
+        <v>0.50104166666666672</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L68">
-        <v>80.900000000000006</v>
+        <v>84.2</v>
       </c>
       <c r="M68">
-        <v>80.900000000000006</v>
+        <v>83.7</v>
       </c>
       <c r="N68">
         <v>29.98</v>
@@ -4479,13 +4445,13 @@
         <v>29.98</v>
       </c>
       <c r="P68">
-        <v>71.5</v>
+        <v>61.5</v>
       </c>
       <c r="Q68">
-        <v>75.2</v>
+        <v>67.5</v>
       </c>
       <c r="T68" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
@@ -4496,10 +4462,10 @@
         <v>105</v>
       </c>
       <c r="C69">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E69" t="s">
         <v>112</v>
@@ -4508,25 +4474,25 @@
         <v>33</v>
       </c>
       <c r="G69">
-        <v>24.3</v>
+        <v>24.1</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69" s="1">
-        <v>0.51388888888888884</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="J69" s="1">
-        <v>0.51527777777777772</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L69">
-        <v>81.8</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="M69">
-        <v>82.5</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="N69">
         <v>29.98</v>
@@ -4535,13 +4501,13 @@
         <v>29.98</v>
       </c>
       <c r="P69">
-        <v>76.900000000000006</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="Q69">
-        <v>81.3</v>
+        <v>73.2</v>
       </c>
       <c r="T69" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
@@ -4552,7 +4518,7 @@
         <v>105</v>
       </c>
       <c r="C70">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
         <v>117</v>
@@ -4570,19 +4536,19 @@
         <v>0</v>
       </c>
       <c r="I70" s="1">
-        <v>0.51736111111111116</v>
+        <v>0.50902777777777775</v>
       </c>
       <c r="J70" s="1">
-        <v>0.51875000000000004</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L70">
-        <v>81.3</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="M70">
-        <v>81</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="N70">
         <v>29.98</v>
@@ -4591,13 +4557,13 @@
         <v>29.98</v>
       </c>
       <c r="P70">
-        <v>74.400000000000006</v>
+        <v>71.5</v>
       </c>
       <c r="Q70">
-        <v>77.5</v>
+        <v>75.2</v>
       </c>
       <c r="T70" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
@@ -4608,10 +4574,10 @@
         <v>105</v>
       </c>
       <c r="C71">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="E71" t="s">
         <v>112</v>
@@ -4620,40 +4586,40 @@
         <v>33</v>
       </c>
       <c r="G71">
-        <v>23.8</v>
+        <v>24.3</v>
       </c>
       <c r="H71">
         <v>0</v>
       </c>
       <c r="I71" s="1">
-        <v>0.52361111111111114</v>
+        <v>0.51388888888888884</v>
       </c>
       <c r="J71" s="1">
-        <v>0.53888888888888886</v>
+        <v>0.51527777777777772</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L71">
-        <v>80</v>
+        <v>81.8</v>
       </c>
       <c r="M71">
-        <v>79.900000000000006</v>
+        <v>82.5</v>
       </c>
       <c r="N71">
         <v>29.98</v>
       </c>
       <c r="O71">
-        <v>29.97</v>
+        <v>29.98</v>
       </c>
       <c r="P71">
-        <v>71.8</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="Q71">
-        <v>74.2</v>
+        <v>81.3</v>
       </c>
       <c r="T71" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
@@ -4664,10 +4630,10 @@
         <v>105</v>
       </c>
       <c r="C72">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="E72" t="s">
         <v>112</v>
@@ -4676,184 +4642,243 @@
         <v>33</v>
       </c>
       <c r="G72">
-        <v>23.9</v>
+        <v>24</v>
       </c>
       <c r="H72">
         <v>0</v>
       </c>
       <c r="I72" s="1">
-        <v>0.53055555555555556</v>
+        <v>0.51736111111111116</v>
       </c>
       <c r="J72" s="1">
-        <v>0.53194444444444444</v>
+        <v>0.51875000000000004</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L72">
-        <v>79.2</v>
+        <v>81.3</v>
       </c>
       <c r="M72">
-        <v>79.2</v>
+        <v>81</v>
       </c>
       <c r="N72">
+        <v>29.98</v>
+      </c>
+      <c r="O72">
+        <v>29.98</v>
+      </c>
+      <c r="P72">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="Q72">
+        <v>77.5</v>
+      </c>
+      <c r="T72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>45233</v>
+      </c>
+      <c r="B73" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" t="s">
+        <v>112</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G73">
+        <v>23.8</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0.52361111111111114</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L73">
+        <v>80</v>
+      </c>
+      <c r="M73">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="N73">
+        <v>29.98</v>
+      </c>
+      <c r="O73">
         <v>29.97</v>
       </c>
-      <c r="O72">
-        <v>29.97</v>
-      </c>
-      <c r="P72">
-        <v>74</v>
-      </c>
-      <c r="Q72">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P73">
+        <v>71.8</v>
+      </c>
+      <c r="Q73">
+        <v>74.2</v>
+      </c>
       <c r="T73" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>124</v>
+      <c r="A74" s="3">
+        <v>45233</v>
       </c>
       <c r="B74" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="E74" t="s">
         <v>112</v>
       </c>
       <c r="F74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G74">
+        <v>23.9</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="J74" s="1">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L74">
+        <v>79.2</v>
+      </c>
+      <c r="M74">
+        <v>79.2</v>
+      </c>
+      <c r="N74">
+        <v>29.97</v>
+      </c>
+      <c r="O74">
+        <v>29.97</v>
+      </c>
+      <c r="P74">
+        <v>74</v>
+      </c>
+      <c r="Q74">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" t="s">
+        <v>125</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>127</v>
+      </c>
+      <c r="E76" t="s">
+        <v>112</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G74">
+      <c r="G76">
         <v>20.6</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H76" t="s">
         <v>131</v>
       </c>
-      <c r="I74" s="1">
+      <c r="I76" s="1">
         <v>0.38958333333333334</v>
       </c>
-      <c r="J74" s="1">
+      <c r="J76" s="1">
         <v>0.43125000000000002</v>
       </c>
-      <c r="K74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T74" s="2" t="s">
+      <c r="K76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T76" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>124</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B77" t="s">
         <v>125</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>126</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D77" t="s">
         <v>128</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E77" t="s">
         <v>112</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G75" t="s">
-        <v>12</v>
-      </c>
-      <c r="H75" t="s">
-        <v>12</v>
-      </c>
-      <c r="I75" s="1">
+      <c r="G77" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77" t="s">
+        <v>12</v>
+      </c>
+      <c r="I77" s="1">
         <v>0.43888888888888888</v>
       </c>
-      <c r="J75" s="1">
+      <c r="J77" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="K75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q75" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B77" t="s">
-        <v>135</v>
-      </c>
-      <c r="C77" t="s">
-        <v>136</v>
-      </c>
-      <c r="D77" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G77">
-        <v>22.3</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77" s="1">
-        <v>0.55902777777777779</v>
-      </c>
-      <c r="J77" s="1">
-        <v>0.56041666666666667</v>
-      </c>
       <c r="K77" s="2" t="s">
         <v>12</v>
       </c>
@@ -4874,59 +4899,6 @@
       </c>
       <c r="Q77" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>134</v>
-      </c>
-      <c r="B78" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78" t="s">
-        <v>137</v>
-      </c>
-      <c r="D78" t="s">
-        <v>145</v>
-      </c>
-      <c r="E78" t="s">
-        <v>13</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G78">
-        <v>21.3</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78" s="1">
-        <v>0.56319444444444444</v>
-      </c>
-      <c r="J78" s="1">
-        <v>0.56458333333333333</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L78">
-        <v>26.7</v>
-      </c>
-      <c r="M78">
-        <v>27.9</v>
-      </c>
-      <c r="N78">
-        <v>1022.9</v>
-      </c>
-      <c r="O78">
-        <v>1023</v>
-      </c>
-      <c r="P78">
-        <v>63.2</v>
-      </c>
-      <c r="Q78">
-        <v>65.599999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
@@ -4937,10 +4909,10 @@
         <v>135</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D79" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="E79" t="s">
         <v>13</v>
@@ -4949,40 +4921,37 @@
         <v>83</v>
       </c>
       <c r="G79">
-        <v>22</v>
+        <v>22.3</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
       <c r="I79" s="1">
-        <v>0.56701388888888893</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="J79" s="1">
-        <v>0.56840277777777781</v>
+        <v>0.56041666666666667</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L79">
-        <v>27</v>
-      </c>
-      <c r="M79">
-        <v>28.1</v>
-      </c>
-      <c r="N79">
-        <v>1023.61</v>
-      </c>
-      <c r="O79">
-        <v>1023</v>
-      </c>
-      <c r="P79">
-        <v>62.5</v>
-      </c>
-      <c r="Q79">
-        <v>67.7</v>
-      </c>
-      <c r="T79" t="s">
-        <v>155</v>
+      <c r="L79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q79" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
@@ -4993,10 +4962,10 @@
         <v>135</v>
       </c>
       <c r="C80" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D80" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E80" t="s">
         <v>13</v>
@@ -5005,25 +4974,25 @@
         <v>83</v>
       </c>
       <c r="G80">
-        <v>23.1</v>
+        <v>21.3</v>
       </c>
       <c r="H80">
         <v>0</v>
       </c>
       <c r="I80" s="1">
-        <v>0.57152777777777775</v>
+        <v>0.56319444444444444</v>
       </c>
       <c r="J80" s="1">
-        <v>0.57291666666666663</v>
+        <v>0.56458333333333333</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L80">
-        <v>26.4</v>
+        <v>26.7</v>
       </c>
       <c r="M80">
-        <v>29.1</v>
+        <v>27.9</v>
       </c>
       <c r="N80">
         <v>1022.9</v>
@@ -5032,13 +5001,10 @@
         <v>1023</v>
       </c>
       <c r="P80">
-        <v>51.3</v>
+        <v>63.2</v>
       </c>
       <c r="Q80">
-        <v>66.8</v>
-      </c>
-      <c r="T80" t="s">
-        <v>156</v>
+        <v>65.599999999999994</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
@@ -5049,10 +5015,10 @@
         <v>135</v>
       </c>
       <c r="C81" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E81" t="s">
         <v>13</v>
@@ -5061,40 +5027,40 @@
         <v>83</v>
       </c>
       <c r="G81">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H81">
         <v>0</v>
       </c>
       <c r="I81" s="1">
-        <v>0.57638888888888884</v>
+        <v>0.56701388888888893</v>
       </c>
       <c r="J81" s="1">
-        <v>0.57777777777777772</v>
+        <v>0.56840277777777781</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L81">
-        <v>26.1</v>
+        <v>27</v>
       </c>
       <c r="M81">
-        <v>27.6</v>
+        <v>28.1</v>
       </c>
       <c r="N81">
-        <v>1022.7</v>
+        <v>1023.61</v>
       </c>
       <c r="O81">
-        <v>1022.8</v>
+        <v>1023</v>
       </c>
       <c r="P81">
-        <v>61.6</v>
+        <v>62.5</v>
       </c>
       <c r="Q81">
-        <v>69.900000000000006</v>
+        <v>67.7</v>
       </c>
       <c r="T81" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
@@ -5105,10 +5071,10 @@
         <v>135</v>
       </c>
       <c r="C82" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D82" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E82" t="s">
         <v>13</v>
@@ -5117,40 +5083,40 @@
         <v>83</v>
       </c>
       <c r="G82">
-        <v>23.5</v>
+        <v>23.1</v>
       </c>
       <c r="H82">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I82" s="1">
-        <v>0.57986111111111116</v>
+        <v>0.57152777777777775</v>
       </c>
       <c r="J82" s="1">
-        <v>0.58125000000000004</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L82">
-        <v>27.6</v>
+        <v>26.4</v>
       </c>
       <c r="M82">
-        <v>28.6</v>
+        <v>29.1</v>
       </c>
       <c r="N82">
-        <v>1022.7</v>
+        <v>1022.9</v>
       </c>
       <c r="O82">
-        <v>1022.7</v>
+        <v>1023</v>
       </c>
       <c r="P82">
-        <v>58.2</v>
+        <v>51.3</v>
       </c>
       <c r="Q82">
-        <v>67.2</v>
+        <v>66.8</v>
       </c>
       <c r="T82" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
@@ -5161,10 +5127,10 @@
         <v>135</v>
       </c>
       <c r="C83" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D83" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E83" t="s">
         <v>13</v>
@@ -5173,40 +5139,40 @@
         <v>83</v>
       </c>
       <c r="G83">
-        <v>21.9</v>
+        <v>21</v>
       </c>
       <c r="H83">
         <v>0</v>
       </c>
       <c r="I83" s="1">
-        <v>0.58368055555555554</v>
+        <v>0.57638888888888884</v>
       </c>
       <c r="J83" s="1">
-        <v>0.58506944444444442</v>
+        <v>0.57777777777777772</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L83">
-        <v>25.3</v>
+        <v>26.1</v>
       </c>
       <c r="M83">
-        <v>27.9</v>
+        <v>27.6</v>
       </c>
       <c r="N83">
-        <v>1022.5</v>
+        <v>1022.7</v>
       </c>
       <c r="O83">
-        <v>1022.7</v>
+        <v>1022.8</v>
       </c>
       <c r="P83">
-        <v>51.1</v>
+        <v>61.6</v>
       </c>
       <c r="Q83">
-        <v>69</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="T83" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
@@ -5217,10 +5183,10 @@
         <v>135</v>
       </c>
       <c r="C84" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D84" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E84" t="s">
         <v>13</v>
@@ -5229,37 +5195,40 @@
         <v>83</v>
       </c>
       <c r="G84">
-        <v>21.7</v>
+        <v>23.5</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I84" s="1">
-        <v>0.58750000000000002</v>
+        <v>0.57986111111111116</v>
       </c>
       <c r="J84" s="1">
-        <v>0.58888888888888891</v>
+        <v>0.58125000000000004</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L84">
-        <v>24.1</v>
+        <v>27.6</v>
       </c>
       <c r="M84">
-        <v>27.1</v>
+        <v>28.6</v>
       </c>
       <c r="N84">
-        <v>1022.6</v>
+        <v>1022.7</v>
       </c>
       <c r="O84">
-        <v>1022.6</v>
+        <v>1022.7</v>
       </c>
       <c r="P84">
-        <v>45.5</v>
+        <v>58.2</v>
       </c>
       <c r="Q84">
-        <v>66.400000000000006</v>
+        <v>67.2</v>
+      </c>
+      <c r="T84" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
@@ -5270,10 +5239,10 @@
         <v>135</v>
       </c>
       <c r="C85" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D85" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E85" t="s">
         <v>13</v>
@@ -5282,22 +5251,22 @@
         <v>83</v>
       </c>
       <c r="G85">
-        <v>21.7</v>
+        <v>21.9</v>
       </c>
       <c r="H85">
         <v>0</v>
       </c>
       <c r="I85" s="1">
-        <v>0.59097222222222223</v>
+        <v>0.58368055555555554</v>
       </c>
       <c r="J85" s="1">
-        <v>0.59236111111111112</v>
+        <v>0.58506944444444442</v>
       </c>
       <c r="K85" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L85">
-        <v>24.5</v>
+        <v>25.3</v>
       </c>
       <c r="M85">
         <v>27.9</v>
@@ -5306,13 +5275,16 @@
         <v>1022.5</v>
       </c>
       <c r="O85">
-        <v>1022.6</v>
+        <v>1022.7</v>
       </c>
       <c r="P85">
-        <v>48</v>
+        <v>51.1</v>
       </c>
       <c r="Q85">
-        <v>68.3</v>
+        <v>69</v>
+      </c>
+      <c r="T85" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
@@ -5323,10 +5295,10 @@
         <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D86" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E86" t="s">
         <v>13</v>
@@ -5335,37 +5307,37 @@
         <v>83</v>
       </c>
       <c r="G86">
-        <v>21.9</v>
+        <v>21.7</v>
       </c>
       <c r="H86">
         <v>0</v>
       </c>
       <c r="I86" s="1">
-        <v>0.59444444444444444</v>
+        <v>0.58750000000000002</v>
       </c>
       <c r="J86" s="1">
-        <v>0.59583333333333333</v>
+        <v>0.58888888888888891</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L86">
-        <v>25.2</v>
+        <v>24.1</v>
       </c>
       <c r="M86">
-        <v>28.4</v>
+        <v>27.1</v>
       </c>
       <c r="N86">
-        <v>1022.4</v>
+        <v>1022.6</v>
       </c>
       <c r="O86">
         <v>1022.6</v>
       </c>
       <c r="P86">
-        <v>52.1</v>
+        <v>45.5</v>
       </c>
       <c r="Q86">
-        <v>66.3</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
@@ -5376,10 +5348,10 @@
         <v>135</v>
       </c>
       <c r="C87" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D87" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E87" t="s">
         <v>13</v>
@@ -5388,25 +5360,25 @@
         <v>83</v>
       </c>
       <c r="G87">
-        <v>21.2</v>
+        <v>21.7</v>
       </c>
       <c r="H87">
         <v>0</v>
       </c>
       <c r="I87" s="1">
-        <v>0.59826388888888893</v>
+        <v>0.59097222222222223</v>
       </c>
       <c r="J87" s="1">
-        <v>0.59965277777777781</v>
+        <v>0.59236111111111112</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L87">
-        <v>25.9</v>
+        <v>24.5</v>
       </c>
       <c r="M87">
-        <v>28.4</v>
+        <v>27.9</v>
       </c>
       <c r="N87">
         <v>1022.5</v>
@@ -5415,123 +5387,120 @@
         <v>1022.6</v>
       </c>
       <c r="P87">
-        <v>44.4</v>
+        <v>48</v>
       </c>
       <c r="Q87">
-        <v>63.3</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="F88" s="2"/>
+      <c r="A88" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88" t="s">
+        <v>143</v>
+      </c>
+      <c r="D88" t="s">
+        <v>153</v>
+      </c>
+      <c r="E88" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G88">
+        <v>21.9</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="J88" s="1">
+        <v>0.59583333333333333</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L88">
+        <v>25.2</v>
+      </c>
+      <c r="M88">
+        <v>28.4</v>
+      </c>
+      <c r="N88">
+        <v>1022.4</v>
+      </c>
+      <c r="O88">
+        <v>1022.6</v>
+      </c>
+      <c r="P88">
+        <v>52.1</v>
+      </c>
+      <c r="Q88">
+        <v>66.3</v>
+      </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C89" t="s">
-        <v>12</v>
-      </c>
-      <c r="D89">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="D89" t="s">
+        <v>154</v>
       </c>
       <c r="E89" t="s">
-        <v>162</v>
+        <v>13</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G89" t="s">
-        <v>12</v>
+        <v>83</v>
+      </c>
+      <c r="G89">
+        <v>21.2</v>
       </c>
       <c r="H89">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I89" s="1">
-        <v>0.46041666666666664</v>
-      </c>
-      <c r="J89" t="s">
-        <v>12</v>
+        <v>0.59826388888888893</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0.59965277777777781</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R89" s="2" t="s">
-        <v>166</v>
+      <c r="L89">
+        <v>25.9</v>
+      </c>
+      <c r="M89">
+        <v>28.4</v>
+      </c>
+      <c r="N89">
+        <v>1022.5</v>
+      </c>
+      <c r="O89">
+        <v>1022.6</v>
+      </c>
+      <c r="P89">
+        <v>44.4</v>
+      </c>
+      <c r="Q89">
+        <v>63.3</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>160</v>
-      </c>
-      <c r="B90" t="s">
-        <v>161</v>
-      </c>
-      <c r="C90" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" t="s">
-        <v>162</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G90" t="s">
-        <v>12</v>
-      </c>
-      <c r="H90" t="s">
-        <v>12</v>
-      </c>
-      <c r="I90" t="s">
-        <v>12</v>
-      </c>
-      <c r="J90" t="s">
-        <v>12</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q90" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
@@ -5543,8 +5512,8 @@
       <c r="C91" t="s">
         <v>12</v>
       </c>
-      <c r="D91" t="s">
-        <v>12</v>
+      <c r="D91">
+        <v>1</v>
       </c>
       <c r="E91" t="s">
         <v>162</v>
@@ -5552,17 +5521,17 @@
       <c r="F91" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G91">
-        <v>28.1</v>
-      </c>
-      <c r="H91" t="s">
-        <v>12</v>
+      <c r="G91" t="s">
+        <v>12</v>
+      </c>
+      <c r="H91">
+        <v>20</v>
       </c>
       <c r="I91" s="1">
-        <v>0.53263888888888888</v>
-      </c>
-      <c r="J91" s="1">
-        <v>0.53472222222222221</v>
+        <v>0.46041666666666664</v>
+      </c>
+      <c r="J91" t="s">
+        <v>12</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>12</v>
@@ -5586,14 +5555,11 @@
         <v>12</v>
       </c>
       <c r="R91" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="T91" t="s">
-        <v>98</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+      <c r="A92" t="s">
         <v>160</v>
       </c>
       <c r="B92" t="s">
@@ -5614,14 +5580,14 @@
       <c r="G92" t="s">
         <v>12</v>
       </c>
-      <c r="H92">
-        <v>2</v>
-      </c>
-      <c r="I92" s="1">
-        <v>0.53819444444444442</v>
-      </c>
-      <c r="J92" s="1">
-        <v>0.54027777777777775</v>
+      <c r="H92" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J92" t="s">
+        <v>12</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>12</v>
@@ -5644,15 +5610,9 @@
       <c r="Q92" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R92" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="T92" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="A93" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B93" t="s">
@@ -5670,17 +5630,17 @@
       <c r="F93" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G93" t="s">
-        <v>12</v>
-      </c>
-      <c r="H93">
-        <v>17</v>
+      <c r="G93">
+        <v>28.1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>12</v>
       </c>
       <c r="I93" s="1">
-        <v>0.54236111111111107</v>
+        <v>0.53263888888888888</v>
       </c>
       <c r="J93" s="1">
-        <v>0.5444444444444444</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>12</v>
@@ -5704,10 +5664,10 @@
         <v>12</v>
       </c>
       <c r="R93" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T93" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
@@ -5733,13 +5693,13 @@
         <v>12</v>
       </c>
       <c r="H94">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="I94" s="1">
-        <v>0.54513888888888884</v>
+        <v>0.53819444444444442</v>
       </c>
       <c r="J94" s="1">
-        <v>0.54722222222222228</v>
+        <v>0.54027777777777775</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>12</v>
@@ -5763,14 +5723,14 @@
         <v>12</v>
       </c>
       <c r="R94" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="T94" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+      <c r="A95" t="s">
         <v>160</v>
       </c>
       <c r="B95" t="s">
@@ -5792,13 +5752,13 @@
         <v>12</v>
       </c>
       <c r="H95">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I95" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.54236111111111107</v>
       </c>
       <c r="J95" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.5444444444444444</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>12</v>
@@ -5822,7 +5782,10 @@
         <v>12</v>
       </c>
       <c r="R95" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+      <c r="T95" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
@@ -5848,13 +5811,13 @@
         <v>12</v>
       </c>
       <c r="H96">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I96" s="1">
-        <v>0.55625000000000002</v>
+        <v>0.54513888888888884</v>
       </c>
       <c r="J96" s="1">
-        <v>0.55833333333333335</v>
+        <v>0.54722222222222228</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>12</v>
@@ -5878,7 +5841,10 @@
         <v>12</v>
       </c>
       <c r="R96" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
+      </c>
+      <c r="T96" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
@@ -5904,13 +5870,13 @@
         <v>12</v>
       </c>
       <c r="H97">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I97" s="1">
-        <v>0.56041666666666667</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J97" s="1">
-        <v>0.56458333333333333</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>12</v>
@@ -5934,11 +5900,11 @@
         <v>12</v>
       </c>
       <c r="R97" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="A98" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B98" t="s">
@@ -5960,13 +5926,13 @@
         <v>12</v>
       </c>
       <c r="H98">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I98" s="1">
-        <v>0.56666666666666665</v>
+        <v>0.55625000000000002</v>
       </c>
       <c r="J98" s="1">
-        <v>0.58750000000000002</v>
+        <v>0.55833333333333335</v>
       </c>
       <c r="K98" s="2" t="s">
         <v>12</v>
@@ -5990,7 +5956,7 @@
         <v>12</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
@@ -6016,13 +5982,13 @@
         <v>12</v>
       </c>
       <c r="H99">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I99" s="1">
-        <v>0.58958333333333335</v>
+        <v>0.56041666666666667</v>
       </c>
       <c r="J99" s="1">
-        <v>0.59652777777777777</v>
+        <v>0.56458333333333333</v>
       </c>
       <c r="K99" s="2" t="s">
         <v>12</v>
@@ -6046,11 +6012,11 @@
         <v>12</v>
       </c>
       <c r="R99" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+      <c r="A100" t="s">
         <v>160</v>
       </c>
       <c r="B100" t="s">
@@ -6075,33 +6041,145 @@
         <v>27</v>
       </c>
       <c r="I100" s="1">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="J100" s="1">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R100" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B101" t="s">
+        <v>161</v>
+      </c>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" t="s">
+        <v>162</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G101" t="s">
+        <v>12</v>
+      </c>
+      <c r="H101">
+        <v>22</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="J101" s="1">
+        <v>0.59652777777777777</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R101" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B102" t="s">
+        <v>161</v>
+      </c>
+      <c r="C102" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" t="s">
+        <v>162</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G102" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102">
+        <v>27</v>
+      </c>
+      <c r="I102" s="1">
         <v>0.6</v>
       </c>
-      <c r="J100" s="1">
+      <c r="J102" s="1">
         <v>0.61041666666666672</v>
       </c>
-      <c r="K100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R100" s="2" t="s">
+      <c r="K102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R102" s="2" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>